<commit_message>
Done Decision Tree A2 - Analysis
</commit_message>
<xml_diff>
--- a/4-Analysis/Decision Tree/DecisionTree A1-test.xlsx
+++ b/4-Analysis/Decision Tree/DecisionTree A1-test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tree" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
-    <t xml:space="preserve">AdaBoost -Test Cases</t>
+    <t xml:space="preserve">Decision Tree -Test Cases</t>
   </si>
   <si>
     <t xml:space="preserve">1.Leaf Instances</t>
@@ -315,7 +315,7 @@
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -354,10 +354,6 @@
     <xf fontId="0" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="4" borderId="3" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="6" borderId="2" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1183,7 +1179,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>9522</xdr:colOff>
+      <xdr:colOff>9521</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -1233,7 +1229,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>9522</xdr:colOff>
+      <xdr:colOff>9521</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -1283,7 +1279,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>9522</xdr:colOff>
+      <xdr:colOff>9521</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>161922</xdr:rowOff>
     </xdr:from>
@@ -1333,7 +1329,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>9522</xdr:colOff>
+      <xdr:colOff>9521</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>180972</xdr:rowOff>
     </xdr:from>
@@ -1383,15 +1379,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>9522</xdr:colOff>
+      <xdr:colOff>9521</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>9522</xdr:rowOff>
+      <xdr:rowOff>9521</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>590547</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>9522</xdr:rowOff>
+      <xdr:rowOff>9521</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -3790,7 +3786,7 @@
       <c r="D24" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="20">
+      <c r="E24" s="6">
         <v>0.89700000000000002</v>
       </c>
     </row>
@@ -4062,7 +4058,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D6" t="s">
@@ -4085,7 +4081,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D7" t="s">
@@ -4187,7 +4183,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D15" t="s">
@@ -4198,7 +4194,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D16" t="s">
@@ -4257,7 +4253,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D23" s="15" t="s">
@@ -4268,13 +4264,13 @@
       </c>
     </row>
     <row r="24">
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="5" t="s">
         <v>43</v>
       </c>
       <c r="D24" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="20">
+      <c r="E24" s="6">
         <v>0.89700000000000002</v>
       </c>
     </row>
@@ -4326,7 +4322,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="B31" s="21" t="s">
+      <c r="B31" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D31" t="s">
@@ -4337,7 +4333,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="5" t="s">
         <v>44</v>
       </c>
       <c r="D32" t="s">

</xml_diff>